<commit_message>
added appoint particular day for duty
</commit_message>
<xml_diff>
--- a/planner_config.xlsx
+++ b/planner_config.xlsx
@@ -262,13 +262,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -714,7 +714,7 @@
   <dimension ref="A1:AI16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -973,8 +973,8 @@
       <c r="C3" s="2">
         <v>0</v>
       </c>
-      <c r="D3" s="2">
-        <v>0</v>
+      <c r="D3" s="8">
+        <v>2</v>
       </c>
       <c r="E3" s="3">
         <v>1</v>
@@ -1015,7 +1015,7 @@
       <c r="Q3" s="2">
         <v>0</v>
       </c>
-      <c r="R3" s="2">
+      <c r="R3" s="9">
         <v>0</v>
       </c>
       <c r="S3" s="2">
@@ -1410,7 +1410,7 @@
       <c r="F7" s="2">
         <v>0</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G7" s="3">
         <v>1</v>
       </c>
       <c r="H7" s="2">
@@ -1428,7 +1428,7 @@
       <c r="L7" s="2">
         <v>0</v>
       </c>
-      <c r="M7" s="9">
+      <c r="M7" s="3">
         <v>1</v>
       </c>
       <c r="N7" s="2">
@@ -1473,7 +1473,7 @@
       <c r="AA7" s="2">
         <v>0</v>
       </c>
-      <c r="AB7" s="8">
+      <c r="AB7" s="3">
         <v>1</v>
       </c>
       <c r="AC7" s="2">
@@ -1615,8 +1615,8 @@
       <c r="C9" s="2">
         <v>0</v>
       </c>
-      <c r="D9" s="2">
-        <v>0</v>
+      <c r="D9" s="8">
+        <v>2</v>
       </c>
       <c r="E9" s="3">
         <v>1</v>
@@ -1657,7 +1657,7 @@
       <c r="Q9" s="2">
         <v>0</v>
       </c>
-      <c r="R9" s="2">
+      <c r="R9" s="9">
         <v>0</v>
       </c>
       <c r="S9" s="2">

</xml_diff>